<commit_message>
Updated G8 ELA data frames To-Do: update UI Complete G5-7 ELA Complete: STE grade analysis
</commit_message>
<xml_diff>
--- a/data/2023ELAItemResults.xlsx
+++ b/data/2023ELAItemResults.xlsx
@@ -960,6 +960,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="4" max="4" width="21.88"/>
+    <col customWidth="1" min="5" max="5" width="121.75"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2096,6 +2097,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="4" max="4" width="21.88"/>
+    <col customWidth="1" min="5" max="5" width="116.25"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3264,6 +3266,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="4" max="4" width="21.88"/>
+    <col customWidth="1" min="5" max="5" width="95.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4432,6 +4435,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="4" max="4" width="21.88"/>
+    <col customWidth="1" min="5" max="5" width="97.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5600,6 +5604,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="4" max="4" width="21.88"/>
+    <col customWidth="1" min="5" max="5" width="97.38"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>